<commit_message>
Better iterative FFT (#6)
* Added command line arguments to Serial program.

* Updated CMakefile in Serial project.

* Better iterative FFT.

* Updated timings.

Co-authored-by: Farooq <farooq@teqniqly.com>
</commit_message>
<xml_diff>
--- a/docs/report/timings.xlsx
+++ b/docs/report/timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\my\COP5522ProjectTeamGold\docs\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C414A5-AAFD-4A78-B8CB-53CAE8760652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4E7AB9-7E75-419B-B27E-62E20E74F6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{31A5E7D5-72B8-4914-B53D-B69F32E9273C}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3509,7 +3509,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C1A29CD-3FC7-4186-B1B2-DB2F4B6D78E9}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C1A29CD-3FC7-4186-B1B2-DB2F4B6D78E9}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -4139,7 +4139,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4175,7 +4175,7 @@
         <v>16</v>
       </c>
       <c r="D2">
-        <v>2.3333300000000002E-3</v>
+        <v>1.33333E-3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -4190,7 +4190,7 @@
         <v>256</v>
       </c>
       <c r="D3">
-        <v>2.7666699999999999E-2</v>
+        <v>3.0333300000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -4205,7 +4205,7 @@
         <v>4096</v>
       </c>
       <c r="D4">
-        <v>0.61899999999999999</v>
+        <v>0.58599999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -4220,7 +4220,7 @@
         <v>65536</v>
       </c>
       <c r="D5">
-        <v>19.972999999999999</v>
+        <v>12.9337</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -4235,7 +4235,7 @@
         <v>1048576</v>
       </c>
       <c r="D6">
-        <v>266.64400000000001</v>
+        <v>239.30199999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -4250,7 +4250,7 @@
         <v>16777216</v>
       </c>
       <c r="D7">
-        <v>4933.2299999999996</v>
+        <v>4717.3599999999997</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -4265,7 +4265,7 @@
         <v>268435456</v>
       </c>
       <c r="D8">
-        <v>196077</v>
+        <v>128852</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -4280,7 +4280,7 @@
         <v>16</v>
       </c>
       <c r="D9">
-        <v>3.33333E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -4295,7 +4295,7 @@
         <v>256</v>
       </c>
       <c r="D10">
-        <v>6.0000000000000001E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -4310,7 +4310,7 @@
         <v>4096</v>
       </c>
       <c r="D11">
-        <v>0.17499999999999999</v>
+        <v>9.9500000000000005E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -4325,7 +4325,7 @@
         <v>65536</v>
       </c>
       <c r="D12">
-        <v>3.7976700000000001</v>
+        <v>1.9016999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -4340,7 +4340,7 @@
         <v>1048576</v>
       </c>
       <c r="D13">
-        <v>72.6267</v>
+        <v>50.888500000000001</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -4355,7 +4355,7 @@
         <v>16777216</v>
       </c>
       <c r="D14">
-        <v>1406.08</v>
+        <v>1113.1199999999999</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -4370,7 +4370,7 @@
         <v>268435456</v>
       </c>
       <c r="D15">
-        <v>26245.599999999999</v>
+        <v>21817.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Iterative/parallel FFT with OpenMP
</commit_message>
<xml_diff>
--- a/docs/report/timings.xlsx
+++ b/docs/report/timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\my\COP5522ProjectTeamGold\docs\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4E7AB9-7E75-419B-B27E-62E20E74F6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A9DC43-F078-4F8C-977D-43B8AAEA99BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{31A5E7D5-72B8-4914-B53D-B69F32E9273C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="21">
   <si>
     <t>Method</t>
   </si>
@@ -65,18 +65,60 @@
   <si>
     <t>Average of Avg Time (ms)</t>
   </si>
+  <si>
+    <t>OpenMP</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Shuffle Time = 6453.98 ms</t>
+  </si>
+  <si>
+    <t>Eval Time = 13691.8 ms</t>
+  </si>
+  <si>
+    <t>For 2^28 items:</t>
+  </si>
+  <si>
+    <t>Inner loop execs</t>
+  </si>
+  <si>
+    <t>Outer loop execs</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Parallel shuffle</t>
+  </si>
+  <si>
+    <t>Parallel shuffle &amp; evaluate</t>
+  </si>
+  <si>
+    <t>https://github.com/rshuston/FFT-C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF808080"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -109,6 +151,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3639,15 +3684,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B250B55E-4437-475B-9216-0CBCA31C9AC0}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0">
-  <autoFilter ref="A1:D15" xr:uid="{B250B55E-4437-475B-9216-0CBCA31C9AC0}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B250B55E-4437-475B-9216-0CBCA31C9AC0}" name="Table1" displayName="Table1" ref="A1:F71" totalsRowShown="0">
+  <autoFilter ref="A1:F71" xr:uid="{B250B55E-4437-475B-9216-0CBCA31C9AC0}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A88AAF9A-B976-4B19-85D5-E2201552F493}" name="Method"/>
+    <tableColumn id="5" xr3:uid="{5C93F350-4415-49CF-B331-D1F46C6436ED}" name="Threads"/>
     <tableColumn id="4" xr3:uid="{66EA5230-DF54-4C9D-8EBA-CEC330AF568E}" name="Power of 2"/>
     <tableColumn id="2" xr3:uid="{11A63F0F-A23A-4BB7-A3F5-AA4848F0836A}" name="N" dataDxfId="0">
       <calculatedColumnFormula>POWER(2, Table1[[#This Row],[Power of 2]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{9CE18878-43B4-4332-A3A3-97BE852BBBC7}" name="Avg Time (ms)"/>
+    <tableColumn id="6" xr3:uid="{20B021E8-A12E-4FA9-8AC9-6D7B4B1209B2}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4136,241 +4183,1499 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE4B4AC-7513-4E02-AD88-5D88B35C6257}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.90625" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>16</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.33333E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>256</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3.0333300000000001E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>4096</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.58599999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>65536</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>12.9337</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>20</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>1048576</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>239.30199999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>24</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>16777216</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>4717.3599999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>268435455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>28</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>268435456</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>128852</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>16</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <f>H7*H8</f>
+        <v>7516192740</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>256</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>4096</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>9.9500000000000005E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>16</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>65536</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1.9016999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G12" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>20</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>1048576</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>50.888500000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>24</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>16777216</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>1113.1199999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
         <v>28</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
         <v>268435456</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>21817.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>256</v>
+      </c>
+      <c r="E17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>4096</v>
+      </c>
+      <c r="E18">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>65536</v>
+      </c>
+      <c r="E19">
+        <v>1.9370000000000001</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>1048576</v>
+      </c>
+      <c r="E20">
+        <v>52.261000000000003</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>24</v>
+      </c>
+      <c r="D21" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16777216</v>
+      </c>
+      <c r="E21">
+        <v>1004.61</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>28</v>
+      </c>
+      <c r="D22" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>268435456</v>
+      </c>
+      <c r="E22">
+        <v>19792.900000000001</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>256</v>
+      </c>
+      <c r="E24">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>4096</v>
+      </c>
+      <c r="E25">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>65536</v>
+      </c>
+      <c r="E26">
+        <v>2.121</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+      <c r="D27" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>1048576</v>
+      </c>
+      <c r="E27">
+        <v>46.765000000000001</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16777216</v>
+      </c>
+      <c r="E28">
+        <v>915.18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>268435456</v>
+      </c>
+      <c r="E29">
+        <v>18420.900000000001</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16</v>
+      </c>
+      <c r="E30">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>256</v>
+      </c>
+      <c r="E31">
+        <v>0.157</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>4096</v>
+      </c>
+      <c r="E32">
+        <v>0.246</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>65536</v>
+      </c>
+      <c r="E33">
+        <v>2.1190000000000002</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>20</v>
+      </c>
+      <c r="D34" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>1048576</v>
+      </c>
+      <c r="E34">
+        <v>43.401000000000003</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>24</v>
+      </c>
+      <c r="D35" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16777216</v>
+      </c>
+      <c r="E35">
+        <v>865.76099999999997</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>28</v>
+      </c>
+      <c r="D36" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>268435456</v>
+      </c>
+      <c r="E36">
+        <v>17058.7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16</v>
+      </c>
+      <c r="E37">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>256</v>
+      </c>
+      <c r="E38">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>4096</v>
+      </c>
+      <c r="E39">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>65536</v>
+      </c>
+      <c r="E40">
+        <v>2.67</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>20</v>
+      </c>
+      <c r="D41" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>1048576</v>
+      </c>
+      <c r="E41">
+        <v>40.753</v>
+      </c>
+      <c r="F41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>24</v>
+      </c>
+      <c r="D42" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16777216</v>
+      </c>
+      <c r="E42">
+        <v>822.82100000000003</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>28</v>
+      </c>
+      <c r="D43" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>268435456</v>
+      </c>
+      <c r="E43">
+        <v>16760.400000000001</v>
+      </c>
+      <c r="F43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16</v>
+      </c>
+      <c r="E44">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>256</v>
+      </c>
+      <c r="E45">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>12</v>
+      </c>
+      <c r="D46" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>4096</v>
+      </c>
+      <c r="E46">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>16</v>
+      </c>
+      <c r="D47" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>65536</v>
+      </c>
+      <c r="E47">
+        <v>2.016</v>
+      </c>
+      <c r="F47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>20</v>
+      </c>
+      <c r="D48" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>1048576</v>
+      </c>
+      <c r="E48">
+        <v>51.542999999999999</v>
+      </c>
+      <c r="F48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>24</v>
+      </c>
+      <c r="D49" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16777216</v>
+      </c>
+      <c r="E49">
+        <v>1013.89</v>
+      </c>
+      <c r="F49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>28</v>
+      </c>
+      <c r="D50" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>268435456</v>
+      </c>
+      <c r="E50">
+        <v>20257.599999999999</v>
+      </c>
+      <c r="F50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16</v>
+      </c>
+      <c r="E51">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="D52" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>256</v>
+      </c>
+      <c r="E52">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>12</v>
+      </c>
+      <c r="D53" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>4096</v>
+      </c>
+      <c r="E53">
+        <v>0.121</v>
+      </c>
+      <c r="F53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <v>16</v>
+      </c>
+      <c r="D54" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>65536</v>
+      </c>
+      <c r="E54">
+        <v>1.282</v>
+      </c>
+      <c r="F54" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>20</v>
+      </c>
+      <c r="D55" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>1048576</v>
+      </c>
+      <c r="E55">
+        <v>32.213000000000001</v>
+      </c>
+      <c r="F55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>24</v>
+      </c>
+      <c r="D56" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16777216</v>
+      </c>
+      <c r="E56">
+        <v>696.87800000000004</v>
+      </c>
+      <c r="F56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>28</v>
+      </c>
+      <c r="D57" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>268435456</v>
+      </c>
+      <c r="E57">
+        <v>17037.599999999999</v>
+      </c>
+      <c r="F57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16</v>
+      </c>
+      <c r="E58">
+        <v>0.12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>8</v>
+      </c>
+      <c r="D59" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>256</v>
+      </c>
+      <c r="E59">
+        <v>0.13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60">
+        <v>12</v>
+      </c>
+      <c r="D60" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>4096</v>
+      </c>
+      <c r="E60">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="F60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <v>16</v>
+      </c>
+      <c r="D61" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>65536</v>
+      </c>
+      <c r="E61">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>1048576</v>
+      </c>
+      <c r="E62">
+        <v>21.841000000000001</v>
+      </c>
+      <c r="F62" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>24</v>
+      </c>
+      <c r="D63" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16777216</v>
+      </c>
+      <c r="E63">
+        <v>460.14499999999998</v>
+      </c>
+      <c r="F63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>28</v>
+      </c>
+      <c r="D64" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>268435456</v>
+      </c>
+      <c r="E64">
+        <v>14015.1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16</v>
+      </c>
+      <c r="E65">
+        <v>0.253</v>
+      </c>
+      <c r="F65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>8</v>
+      </c>
+      <c r="D66" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>256</v>
+      </c>
+      <c r="E66">
+        <v>1.609</v>
+      </c>
+      <c r="F66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>12</v>
+      </c>
+      <c r="D67" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>4096</v>
+      </c>
+      <c r="E67">
+        <v>1.6639999999999999</v>
+      </c>
+      <c r="F67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <v>16</v>
+      </c>
+      <c r="D68" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>65536</v>
+      </c>
+      <c r="E68">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="F68" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69">
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <v>20</v>
+      </c>
+      <c r="D69" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>1048576</v>
+      </c>
+      <c r="E69">
+        <v>14.919</v>
+      </c>
+      <c r="F69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>24</v>
+      </c>
+      <c r="D70" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>16777216</v>
+      </c>
+      <c r="E70">
+        <v>450.65199999999999</v>
+      </c>
+      <c r="F70" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71">
+        <v>8</v>
+      </c>
+      <c r="C71">
+        <v>28</v>
+      </c>
+      <c r="D71" s="4">
+        <f>POWER(2, Table1[[#This Row],[Power of 2]])</f>
+        <v>268435456</v>
+      </c>
+      <c r="E71">
+        <v>13614.3</v>
+      </c>
+      <c r="F71" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>